<commit_message>
feat: test scenario consultation
</commit_message>
<xml_diff>
--- a/configuration/InstructorConsultationData.xlsx
+++ b/configuration/InstructorConsultationData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ryu\github\SoftwareTesting\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF3F70F-1536-406C-BF61-2352045672AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D4E8B8-A29F-4039-9C00-23D05B00AB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{B9A3D592-CF39-4016-87BE-195989F8B0B0}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="16200" windowHeight="9308" xr2:uid="{B9A3D592-CF39-4016-87BE-195989F8B0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -103,6 +103,21 @@
   </si>
   <si>
     <t>All Over The World</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>In Person</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>10:08</t>
+  </si>
+  <si>
+    <t>12:08</t>
   </si>
 </sst>
 </file>
@@ -461,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CDB5AC-CEE9-403E-BDDE-463CBE6DD5D0}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -566,6 +581,35 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>